<commit_message>
Grid Routine 통합전 commit
</commit_message>
<xml_diff>
--- a/MS_FVM/Result/Post/OrderTest.xlsx
+++ b/MS_FVM/Result/Post/OrderTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KimMinSeok\source\repos\MS_FVM\MS_FVM\RSC\Post\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KimMinSeok\source\repos\MS_FVM\MS_FVM\Result\Post\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8818E9-9B1B-489E-9265-8290E3A9A571}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA2C95C-F820-45AF-A69E-F7CEB6F2E804}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{1CFF3398-A0ED-430E-B466-1E9E1EEDD2C1}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="B6:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G8" sqref="G8:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>